<commit_message>
router update and new tester routers added
</commit_message>
<xml_diff>
--- a/templates/soldering.xlsx
+++ b/templates/soldering.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react projects\nokia\git\Nokia-API\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react projects\nokia\Nokia-DWS-main\Backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A0C65C-FDC0-411B-A43D-0B3198A2A2DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5425544B-6A84-4376-9B65-D240B47A4345}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,14 +116,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -136,10 +155,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,34 +488,34 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -510,81 +526,81 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="8" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>